<commit_message>
Fire/Ice Bullet, Barrier & Turret Added
</commit_message>
<xml_diff>
--- a/工作表.xlsx
+++ b/工作表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>项目名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -169,15 +169,7 @@
     <t>仓库+快捷栏两个面板</t>
   </si>
   <si>
-    <t>防护罩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>炮台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>杂项特效</t>
+    <t>防护罩、炮台</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -185,7 +177,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +195,13 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,11 +239,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -525,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -557,12 +557,16 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -579,18 +583,24 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -606,6 +616,7 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
+      <c r="C11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -617,6 +628,7 @@
       <c r="B13" t="s">
         <v>15</v>
       </c>
+      <c r="C13" s="2"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -653,91 +665,82 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>23</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>29</v>
-      </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>33</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>35</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>